<commit_message>
Changes on wait and removed invalid login test case
</commit_message>
<xml_diff>
--- a/workspace/MobiliyaAppiumFramework/bin/com/mobiliya/edvelop/testData/TestData.xlsx
+++ b/workspace/MobiliyaAppiumFramework/bin/com/mobiliya/edvelop/testData/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t xml:space="preserve">Username / Email</t>
   </si>
@@ -35,10 +35,10 @@
     <t xml:space="preserve">AgreeYa@123</t>
   </si>
   <si>
-    <t xml:space="preserve">kanika00@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">agreeya00</t>
+    <t xml:space="preserve">mobiliya1234@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mobiliya123</t>
   </si>
 </sst>
 </file>
@@ -137,15 +137,15 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.3469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.5816326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -180,17 +180,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="12.9591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -203,24 +203,9 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>